<commit_message>
Fix news fetcher extraction logic and add new news item
- Fixed extraction function to properly parse Perplexity API research responses
- Improved prompt clarity and JSON parsing for news items
- Changed extraction model to 'sonar' for faster, more reliable extraction
- Added better error handling and logging for debugging
- Discovered new company: Farrel Pomini
- Added news item #26: Farrel Pomini innovation announcement (Nov 21, 2025)
- Generated Hugo story for ID #26

🤖 Generated with Claude Code

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/companies.xlsx
+++ b/companies.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q52"/>
+  <dimension ref="A1:Q53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,11 +456,7 @@
     <col width="12" customWidth="1" min="8" max="8"/>
     <col width="15" customWidth="1" min="9" max="9"/>
     <col width="15" customWidth="1" min="10" max="10"/>
-    <col width="35" customWidth="1" min="11" max="11"/>
-    <col width="35" customWidth="1" min="12" max="12"/>
-    <col width="35" customWidth="1" min="13" max="13"/>
-    <col width="35" customWidth="1" min="14" max="14"/>
-    <col width="15" customWidth="1" min="15" max="15"/>
+    <col width="15" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -601,7 +597,7 @@
           <t>2025-10-30</t>
         </is>
       </c>
-      <c r="M2" s="2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>https://www.natureworksllc.com/about-natureworks/news</t>
         </is>
@@ -663,12 +659,12 @@
           <t>2025-10-30</t>
         </is>
       </c>
-      <c r="M3" s="2" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>https://www.basf.com/ch/fr/media</t>
         </is>
       </c>
-      <c r="N3" s="2" t="inlineStr">
+      <c r="N3" t="inlineStr">
         <is>
           <t>https://twitter.com/BASF</t>
         </is>
@@ -735,7 +731,7 @@
           <t>2025-10-30</t>
         </is>
       </c>
-      <c r="M4" s="2" t="inlineStr">
+      <c r="M4" t="inlineStr">
         <is>
           <t>http://www.novamont.com/news</t>
         </is>
@@ -807,12 +803,12 @@
           <t>2025-10-30</t>
         </is>
       </c>
-      <c r="M5" s="2" t="inlineStr">
+      <c r="M5" t="inlineStr">
         <is>
           <t>https://www.corbion.com/en/media</t>
         </is>
       </c>
-      <c r="N5" s="2" t="inlineStr">
+      <c r="N5" t="inlineStr">
         <is>
           <t>https://twitter.com/Corbion</t>
         </is>
@@ -884,7 +880,7 @@
           <t>2025-10-30</t>
         </is>
       </c>
-      <c r="L6" s="2" t="inlineStr">
+      <c r="L6" t="inlineStr">
         <is>
           <t>https://biomebioplastics.com/feed/</t>
         </is>
@@ -956,12 +952,12 @@
           <t>2025-10-30</t>
         </is>
       </c>
-      <c r="L7" s="2" t="inlineStr">
+      <c r="L7" t="inlineStr">
         <is>
           <t>https://www.danimerscientific.com/feed</t>
         </is>
       </c>
-      <c r="N7" s="2" t="inlineStr">
+      <c r="N7" t="inlineStr">
         <is>
           <t>https://twitter.com/DanimerScientif</t>
         </is>
@@ -1028,7 +1024,7 @@
           <t>2025-10-30</t>
         </is>
       </c>
-      <c r="N8" s="2" t="inlineStr">
+      <c r="N8" t="inlineStr">
         <is>
           <t>https://twitter.com/TotalEnergies</t>
         </is>
@@ -1100,12 +1096,12 @@
           <t>2025-10-30</t>
         </is>
       </c>
-      <c r="M9" s="2" t="inlineStr">
+      <c r="M9" t="inlineStr">
         <is>
           <t>https://www.mcgc.com#newsRelease</t>
         </is>
       </c>
-      <c r="N9" s="2" t="inlineStr">
+      <c r="N9" t="inlineStr">
         <is>
           <t>https://twitter.com/MitsubishiChem</t>
         </is>
@@ -1229,12 +1225,12 @@
           <t>2025-10-30</t>
         </is>
       </c>
-      <c r="L11" s="2" t="inlineStr">
+      <c r="L11" t="inlineStr">
         <is>
           <t>https://www.futerro.com/feed/</t>
         </is>
       </c>
-      <c r="M11" s="2" t="inlineStr">
+      <c r="M11" t="inlineStr">
         <is>
           <t>https://www.futerro.com/news-media/news/</t>
         </is>
@@ -1296,7 +1292,7 @@
           <t>2025-10-30</t>
         </is>
       </c>
-      <c r="N12" s="2" t="inlineStr">
+      <c r="N12" t="inlineStr">
         <is>
           <t>https://twitter.com/BioOnBioplastic</t>
         </is>
@@ -1368,12 +1364,12 @@
           <t>2025-10-30</t>
         </is>
       </c>
-      <c r="M13" s="2" t="inlineStr">
+      <c r="M13" t="inlineStr">
         <is>
           <t>https://www.braskem.com/europe/news</t>
         </is>
       </c>
-      <c r="N13" s="2" t="inlineStr">
+      <c r="N13" t="inlineStr">
         <is>
           <t>https://twitter.com/Braskem</t>
         </is>
@@ -1616,7 +1612,7 @@
           <t>2025-10-30</t>
         </is>
       </c>
-      <c r="M17" s="2" t="inlineStr">
+      <c r="M17" t="inlineStr">
         <is>
           <t>https://www.ti-films.com</t>
         </is>
@@ -1683,7 +1679,7 @@
           <t>2025-10-30</t>
         </is>
       </c>
-      <c r="N18" s="2" t="inlineStr">
+      <c r="N18" t="inlineStr">
         <is>
           <t>https://twitter.com/AmcorLimited</t>
         </is>
@@ -1755,7 +1751,7 @@
           <t>2025-10-30</t>
         </is>
       </c>
-      <c r="M19" s="2" t="inlineStr">
+      <c r="M19" t="inlineStr">
         <is>
           <t>https://www.erema.com/de/impressum/</t>
         </is>
@@ -1874,7 +1870,7 @@
           <t>2025-10-30</t>
         </is>
       </c>
-      <c r="M21" s="2" t="inlineStr">
+      <c r="M21" t="inlineStr">
         <is>
           <t>https://www.palsgaard.com/en/about-us/news-about-palsgaard/</t>
         </is>
@@ -1936,12 +1932,12 @@
           <t>2025-10-30</t>
         </is>
       </c>
-      <c r="L22" s="2" t="inlineStr">
+      <c r="L22" t="inlineStr">
         <is>
           <t>https://cjbiomaterials.com/feed/</t>
         </is>
       </c>
-      <c r="M22" s="2" t="inlineStr">
+      <c r="M22" t="inlineStr">
         <is>
           <t>https://cjbiomaterials.com/about/news/</t>
         </is>
@@ -2003,12 +1999,12 @@
           <t>2025-10-30</t>
         </is>
       </c>
-      <c r="M23" s="2" t="inlineStr">
+      <c r="M23" t="inlineStr">
         <is>
           <t>https://www.packaginginsights.com/news.html</t>
         </is>
       </c>
-      <c r="N23" s="2" t="inlineStr">
+      <c r="N23" t="inlineStr">
         <is>
           <t>https://twitter.com/PackagingInsight</t>
         </is>
@@ -2075,12 +2071,12 @@
           <t>2025-10-30</t>
         </is>
       </c>
-      <c r="L24" s="2" t="inlineStr">
+      <c r="L24" t="inlineStr">
         <is>
           <t>https://www.greendotbioplastics.com/home/feed/</t>
         </is>
       </c>
-      <c r="M24" s="2" t="inlineStr">
+      <c r="M24" t="inlineStr">
         <is>
           <t>https://www.greendotbioplastics.com/news/</t>
         </is>
@@ -2147,7 +2143,7 @@
           <t>2025-10-30</t>
         </is>
       </c>
-      <c r="M25" s="2" t="inlineStr">
+      <c r="M25" t="inlineStr">
         <is>
           <t>https://www.kaneka.co.jp/en/topics/</t>
         </is>
@@ -2214,12 +2210,12 @@
           <t>2025-10-30</t>
         </is>
       </c>
-      <c r="L26" s="2" t="inlineStr">
+      <c r="L26" t="inlineStr">
         <is>
           <t>https://oneworldproducts.com/feed/</t>
         </is>
       </c>
-      <c r="M26" s="2" t="inlineStr">
+      <c r="M26" t="inlineStr">
         <is>
           <t>https://oneworldproducts.com/news/</t>
         </is>
@@ -2338,7 +2334,7 @@
           <t>2025-10-30</t>
         </is>
       </c>
-      <c r="N28" s="2" t="inlineStr">
+      <c r="N28" t="inlineStr">
         <is>
           <t>https://twitter.com/BerryGlobal</t>
         </is>
@@ -2410,7 +2406,7 @@
           <t>2025-10-30</t>
         </is>
       </c>
-      <c r="L29" s="2" t="inlineStr">
+      <c r="L29" t="inlineStr">
         <is>
           <t>https://sanisure.com/feed</t>
         </is>
@@ -2472,7 +2468,7 @@
           <t>2025-10-30</t>
         </is>
       </c>
-      <c r="N30" s="2" t="inlineStr">
+      <c r="N30" t="inlineStr">
         <is>
           <t>https://twitter.com/RoquetteGroup</t>
         </is>
@@ -2549,12 +2545,12 @@
           <t>2025-10-30</t>
         </is>
       </c>
-      <c r="M31" s="2" t="inlineStr">
+      <c r="M31" t="inlineStr">
         <is>
           <t>https://www.basf.com/ch/fr/media</t>
         </is>
       </c>
-      <c r="N31" s="2" t="inlineStr">
+      <c r="N31" t="inlineStr">
         <is>
           <t>https://twitter.com/BASF</t>
         </is>
@@ -2631,12 +2627,12 @@
           <t>2025-11-05</t>
         </is>
       </c>
-      <c r="L32" s="2" t="inlineStr">
+      <c r="L32" t="inlineStr">
         <is>
           <t>https://www.verdebioresins.com/feed</t>
         </is>
       </c>
-      <c r="M32" s="2" t="inlineStr">
+      <c r="M32" t="inlineStr">
         <is>
           <t>https://www.verdebioresins.com/news/</t>
         </is>
@@ -2703,12 +2699,12 @@
           <t>2025-11-05</t>
         </is>
       </c>
-      <c r="M33" s="2" t="inlineStr">
+      <c r="M33" t="inlineStr">
         <is>
           <t>https://global.honda/en/newsroom/?from=top_text_btn</t>
         </is>
       </c>
-      <c r="N33" s="2" t="inlineStr">
+      <c r="N33" t="inlineStr">
         <is>
           <t>https://twitter.com/Honda</t>
         </is>
@@ -2785,12 +2781,12 @@
           <t>2025-11-05</t>
         </is>
       </c>
-      <c r="M34" s="2" t="inlineStr">
+      <c r="M34" t="inlineStr">
         <is>
           <t>https://www.sabic.com/en/newsandmedia</t>
         </is>
       </c>
-      <c r="N34" s="2" t="inlineStr">
+      <c r="N34" t="inlineStr">
         <is>
           <t>https://twitter.com/SABIC_Careers</t>
         </is>
@@ -2909,12 +2905,12 @@
           <t>2025-11-07</t>
         </is>
       </c>
-      <c r="L36" s="2" t="inlineStr">
+      <c r="L36" t="inlineStr">
         <is>
           <t>https://www.rwdc-industries.com/feed/rss2</t>
         </is>
       </c>
-      <c r="M36" s="2" t="inlineStr">
+      <c r="M36" t="inlineStr">
         <is>
           <t>https://www.rwdc-industries.com</t>
         </is>
@@ -2981,12 +2977,12 @@
           <t>2025-11-07</t>
         </is>
       </c>
-      <c r="L37" s="2" t="inlineStr">
+      <c r="L37" t="inlineStr">
         <is>
           <t>https://www.genomatica.com/home/feed/</t>
         </is>
       </c>
-      <c r="M37" s="2" t="inlineStr">
+      <c r="M37" t="inlineStr">
         <is>
           <t>https://www.genomatica.com/news/</t>
         </is>
@@ -3115,7 +3111,7 @@
           <t>2025-11-07</t>
         </is>
       </c>
-      <c r="M39" s="2" t="inlineStr">
+      <c r="M39" t="inlineStr">
         <is>
           <t>https://www.granulous.com/blog</t>
         </is>
@@ -3172,12 +3168,12 @@
           <t>2025-11-07</t>
         </is>
       </c>
-      <c r="L40" s="2" t="inlineStr">
+      <c r="L40" t="inlineStr">
         <is>
           <t>https://www.blueoceanclosures.com/feed/</t>
         </is>
       </c>
-      <c r="M40" s="2" t="inlineStr">
+      <c r="M40" t="inlineStr">
         <is>
           <t>https://www.blueoceanclosures.com/news/</t>
         </is>
@@ -3861,108 +3857,70 @@
           <t>2025-11-19</t>
         </is>
       </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Farrel Pomini</t>
+        </is>
+      </c>
+      <c r="E53" s="3" t="inlineStr"/>
+      <c r="F53" s="3" t="inlineStr"/>
+      <c r="G53" s="3" t="inlineStr"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D2" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M2" r:id="rId2"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D3" r:id="rId3"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M3" r:id="rId4"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N3" r:id="rId5"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D4" r:id="rId6"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M4" r:id="rId7"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D5" r:id="rId8"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M5" r:id="rId9"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N5" r:id="rId10"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D6" r:id="rId11"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="L6" r:id="rId12"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D7" r:id="rId13"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="L7" r:id="rId14"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N7" r:id="rId15"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D8" r:id="rId16"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N8" r:id="rId17"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D9" r:id="rId18"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M9" r:id="rId19"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N9" r:id="rId20"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D10" r:id="rId21"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D11" r:id="rId22"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="L11" r:id="rId23"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M11" r:id="rId24"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D12" r:id="rId25"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N12" r:id="rId26"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D13" r:id="rId27"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M13" r:id="rId28"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N13" r:id="rId29"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D14" r:id="rId30"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D15" r:id="rId31"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D16" r:id="rId32"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D17" r:id="rId33"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M17" r:id="rId34"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D18" r:id="rId35"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N18" r:id="rId36"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D19" r:id="rId37"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M19" r:id="rId38"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D20" r:id="rId39"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D21" r:id="rId40"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M21" r:id="rId41"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D22" r:id="rId42"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="L22" r:id="rId43"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M22" r:id="rId44"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D23" r:id="rId45"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M23" r:id="rId46"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N23" r:id="rId47"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D24" r:id="rId48"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="L24" r:id="rId49"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M24" r:id="rId50"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D25" r:id="rId51"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M25" r:id="rId52"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D26" r:id="rId53"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="L26" r:id="rId54"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M26" r:id="rId55"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D27" r:id="rId56"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D28" r:id="rId57"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N28" r:id="rId58"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D29" r:id="rId59"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="L29" r:id="rId60"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D30" r:id="rId61"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N30" r:id="rId62"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D31" r:id="rId63"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M31" r:id="rId64"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N31" r:id="rId65"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D32" r:id="rId66"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="L32" r:id="rId67"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M32" r:id="rId68"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D33" r:id="rId69"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M33" r:id="rId70"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N33" r:id="rId71"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D34" r:id="rId72"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M34" r:id="rId73"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N34" r:id="rId74"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D35" r:id="rId75"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D36" r:id="rId76"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="L36" r:id="rId77"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M36" r:id="rId78"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D37" r:id="rId79"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="L37" r:id="rId80"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M37" r:id="rId81"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D38" r:id="rId82"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D39" r:id="rId83"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M39" r:id="rId84"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D40" r:id="rId85"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="L40" r:id="rId86"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M40" r:id="rId87"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D41" r:id="rId88"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D42" r:id="rId89"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D43" r:id="rId90"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D44" r:id="rId91"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D45" r:id="rId92"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D46" r:id="rId93"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D47" r:id="rId94"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D48" r:id="rId95"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D49" r:id="rId96"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D50" r:id="rId97"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D51" r:id="rId98"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D52" r:id="rId99"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D3" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D4" r:id="rId3"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D5" r:id="rId4"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D6" r:id="rId5"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D7" r:id="rId6"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D8" r:id="rId7"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D9" r:id="rId8"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D10" r:id="rId9"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D11" r:id="rId10"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D12" r:id="rId11"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D13" r:id="rId12"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D14" r:id="rId13"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D15" r:id="rId14"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D16" r:id="rId15"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D17" r:id="rId16"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D18" r:id="rId17"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D19" r:id="rId18"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D20" r:id="rId19"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D21" r:id="rId20"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D22" r:id="rId21"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D23" r:id="rId22"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D24" r:id="rId23"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D25" r:id="rId24"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D26" r:id="rId25"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D27" r:id="rId26"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D28" r:id="rId27"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D29" r:id="rId28"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D30" r:id="rId29"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D31" r:id="rId30"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D32" r:id="rId31"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D33" r:id="rId32"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D34" r:id="rId33"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D35" r:id="rId34"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D36" r:id="rId35"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D37" r:id="rId36"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D38" r:id="rId37"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D39" r:id="rId38"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D40" r:id="rId39"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D41" r:id="rId40"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D42" r:id="rId41"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D43" r:id="rId42"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D44" r:id="rId43"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D45" r:id="rId44"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D46" r:id="rId45"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D47" r:id="rId46"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D48" r:id="rId47"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D49" r:id="rId48"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D50" r:id="rId49"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D51" r:id="rId50"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D52" r:id="rId51"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>